<commit_message>
Test: updated headers of all HMRC examples
</commit_message>
<xml_diff>
--- a/test/HMRC-Examples/CRYPTO22251.xlsx
+++ b/test/HMRC-Examples/CRYPTO22251.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottgreen/Development/BittyTaxRelease/BittyTax/test/HMRC-examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottgreen/Development/BittyTax/test/HMRC-Examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1853D7EE-3C17-CD43-81DC-3AFEE36BB301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7464385-3A4F-C046-9B19-A2B5A90D8807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15720" yWindow="6760" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22760" yWindow="3620" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRYPTO22251" sheetId="2" r:id="rId1"/>
@@ -37,27 +37,18 @@
     <t>Buy Asset</t>
   </si>
   <si>
-    <t>Buy Value</t>
-  </si>
-  <si>
     <t>Sell Quantity</t>
   </si>
   <si>
     <t>Sell Asset</t>
   </si>
   <si>
-    <t>Sell Value</t>
-  </si>
-  <si>
     <t>Fee Quantity</t>
   </si>
   <si>
     <t>Fee Asset</t>
   </si>
   <si>
-    <t>Fee Value</t>
-  </si>
-  <si>
     <t>Wallet</t>
   </si>
   <si>
@@ -86,6 +77,15 @@
   </si>
   <si>
     <t>On 1 December 20XX Victoria sells 50 of her token A for £300,000.</t>
+  </si>
+  <si>
+    <t>Buy Value in GBP</t>
+  </si>
+  <si>
+    <t>Sell Value in GBP</t>
+  </si>
+  <si>
+    <t>Fee Value in GBP</t>
   </si>
 </sst>
 </file>
@@ -143,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -151,27 +151,82 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -235,21 +290,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00A62E9D-CE53-9242-A60A-605A9B7D0BBF}" name="Coinbase3" displayName="Coinbase3" ref="A1:M6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00A62E9D-CE53-9242-A60A-605A9B7D0BBF}" name="Coinbase3" displayName="Coinbase3" ref="A1:M6" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1">
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{C4250C2B-4A12-2248-B34A-C4F79251FE77}" name="Type"/>
     <tableColumn id="2" xr3:uid="{5EBD8BA2-CB0D-AB4E-8761-924749F76E93}" name="Buy Quantity"/>
     <tableColumn id="3" xr3:uid="{466819A5-0311-D244-AC85-A1D10F935994}" name="Buy Asset"/>
-    <tableColumn id="4" xr3:uid="{50A9BE12-41FE-6D4E-8EEB-212469747E0C}" name="Buy Value"/>
+    <tableColumn id="4" xr3:uid="{50A9BE12-41FE-6D4E-8EEB-212469747E0C}" name="Buy Value in GBP"/>
     <tableColumn id="5" xr3:uid="{48D6E9FA-985C-0445-95CE-2FE0D8C34BEB}" name="Sell Quantity"/>
     <tableColumn id="6" xr3:uid="{C01909FF-C440-8F42-B9D0-9D2CC72661C6}" name="Sell Asset"/>
-    <tableColumn id="7" xr3:uid="{1389A432-9869-C44A-A7D5-B8518E118556}" name="Sell Value"/>
+    <tableColumn id="7" xr3:uid="{1389A432-9869-C44A-A7D5-B8518E118556}" name="Sell Value in GBP"/>
     <tableColumn id="8" xr3:uid="{4DE3AD94-3B46-5A43-ACA9-57A2EA02C455}" name="Fee Quantity"/>
     <tableColumn id="9" xr3:uid="{E9825626-CFFA-AD44-A5FC-4BD707717C89}" name="Fee Asset"/>
-    <tableColumn id="10" xr3:uid="{13B33C37-F409-C547-8677-DD8E263F3DFC}" name="Fee Value"/>
+    <tableColumn id="10" xr3:uid="{13B33C37-F409-C547-8677-DD8E263F3DFC}" name="Fee Value in GBP"/>
     <tableColumn id="11" xr3:uid="{ACB36948-A178-4645-8219-1955AE354070}" name="Wallet"/>
     <tableColumn id="12" xr3:uid="{0C3B0D29-5308-A74C-9493-21C5C975244B}" name="Timestamp"/>
-    <tableColumn id="13" xr3:uid="{44422ED6-6FBD-3347-ABA1-F563FD4BAB7A}" name="Note" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{44422ED6-6FBD-3347-ABA1-F563FD4BAB7A}" name="Note" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -580,7 +635,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,242 +643,242 @@
     <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="67.83203125" customWidth="1"/>
+    <col min="13" max="13" width="68.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>17</v>
+      <c r="M1" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="6" t="s">
-        <v>18</v>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
         <v>126000</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="5">
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="4">
         <v>43831</v>
       </c>
-      <c r="M3" s="6"/>
+      <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>100</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="4">
+        <v>43831</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3">
-        <v>1000</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="5">
-        <v>43831</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>50</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3">
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="2">
         <v>125000</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="5">
+      <c r="G5" s="3"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="4">
         <v>44092</v>
       </c>
-      <c r="M5" s="5" t="s">
-        <v>20</v>
+      <c r="M5" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>300000</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3">
+      <c r="D6" s="3"/>
+      <c r="E6" s="2">
         <v>50</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="5">
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="4">
         <v>44166</v>
       </c>
-      <c r="M6" s="5" t="s">
-        <v>21</v>
+      <c r="M6" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4 B6">
-    <cfRule type="expression" dxfId="10" priority="14">
+    <cfRule type="expression" dxfId="12" priority="14">
       <formula>INT(B4)=B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="expression" dxfId="9" priority="15">
+    <cfRule type="expression" dxfId="11" priority="15">
       <formula>INT(E4)=E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4 H6">
-    <cfRule type="expression" dxfId="8" priority="16">
+    <cfRule type="expression" dxfId="10" priority="16">
       <formula>INT(H4)=H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="7" priority="13">
+    <cfRule type="expression" dxfId="9" priority="13">
       <formula>INT(E6)=E6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>INT(B3)=B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>INT(E3)=E3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>INT(H3)=H3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>INT(B5)=B5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>INT(E5)=E5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>INT(H5)=H5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>